<commit_message>
testing functions for GUI
</commit_message>
<xml_diff>
--- a/Manga database.xlsx
+++ b/Manga database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tj\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE1B5B5-9FC7-4A2C-9C08-334DB32D6F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C9A54A-FA57-494C-9D0B-2FD498BC695F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1590" windowWidth="24240" windowHeight="13140" xr2:uid="{0A906560-0927-4CDC-89CC-53F22AA99BE7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="228">
   <si>
     <t xml:space="preserve">Serialization </t>
   </si>
@@ -700,9 +700,6 @@
   </si>
   <si>
     <t>https://mangadex.org/title/136c516e-a9dd-411b-93b7-2f5c78be4ae8</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>Arisou de NASA-sou</t>
@@ -757,14 +754,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Symbol"/>
-      <family val="1"/>
-      <charset val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -773,6 +762,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -918,7 +915,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -940,9 +937,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -952,11 +946,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1391,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C00074A-E8E9-4DA5-8870-A82B806B5323}">
   <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="K115" sqref="K115"/>
+    <sheetView tabSelected="1" topLeftCell="B80" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,8 +1467,8 @@
       <c r="I2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>220</v>
+      <c r="J2" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>32</v>
@@ -1503,8 +1500,8 @@
       <c r="I3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>220</v>
+      <c r="J3" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>32</v>
@@ -1532,8 +1529,8 @@
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="7" t="s">
-        <v>220</v>
+      <c r="J4" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>32</v>
@@ -1563,8 +1560,8 @@
         <v>149</v>
       </c>
       <c r="I5" s="5"/>
-      <c r="J5" s="7" t="s">
-        <v>220</v>
+      <c r="J5" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>32</v>
@@ -1596,8 +1593,8 @@
       <c r="I6" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>220</v>
+      <c r="J6" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>32</v>
@@ -1627,8 +1624,8 @@
         <v>27</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="J7" s="7" t="s">
-        <v>220</v>
+      <c r="J7" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>32</v>
@@ -1660,8 +1657,8 @@
       <c r="I8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>220</v>
+      <c r="J8" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>32</v>
@@ -1693,8 +1690,8 @@
       <c r="I9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>220</v>
+      <c r="J9" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>32</v>
@@ -1726,46 +1723,46 @@
       <c r="I10" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="11">
-        <v>0</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1790,8 +1787,8 @@
       <c r="I12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="7" t="s">
-        <v>220</v>
+      <c r="J12" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>32</v>
@@ -1823,8 +1820,8 @@
       <c r="I13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="7" t="s">
-        <v>220</v>
+      <c r="J13" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>32</v>
@@ -1856,8 +1853,8 @@
       <c r="I14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="7" t="s">
-        <v>220</v>
+      <c r="J14" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>32</v>
@@ -1889,8 +1886,8 @@
       <c r="I15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="7" t="s">
-        <v>220</v>
+      <c r="J15" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K15" s="5" t="s">
         <v>32</v>
@@ -1922,8 +1919,8 @@
       <c r="I16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="7" t="s">
-        <v>220</v>
+      <c r="J16" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K16" s="5" t="s">
         <v>32</v>
@@ -1955,43 +1952,43 @@
       <c r="I17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="11">
-        <v>0</v>
-      </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="K18" s="11" t="s">
+      <c r="K18" s="10" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2021,8 +2018,8 @@
       <c r="I19" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J19" s="7" t="s">
-        <v>220</v>
+      <c r="J19" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>32</v>
@@ -2048,8 +2045,8 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="7" t="s">
-        <v>220</v>
+      <c r="J20" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>32</v>
@@ -2081,8 +2078,8 @@
       <c r="I21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J21" s="7" t="s">
-        <v>220</v>
+      <c r="J21" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>32</v>
@@ -2112,8 +2109,8 @@
         <v>218</v>
       </c>
       <c r="I22" s="5"/>
-      <c r="J22" s="7" t="s">
-        <v>220</v>
+      <c r="J22" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>32</v>
@@ -2143,8 +2140,8 @@
         <v>17</v>
       </c>
       <c r="I23" s="5"/>
-      <c r="J23" s="7" t="s">
-        <v>220</v>
+      <c r="J23" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>32</v>
@@ -2176,8 +2173,8 @@
       <c r="I24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="7" t="s">
-        <v>220</v>
+      <c r="J24" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>32</v>
@@ -2209,8 +2206,8 @@
       <c r="I25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="7" t="s">
-        <v>220</v>
+      <c r="J25" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>32</v>
@@ -2242,8 +2239,8 @@
       <c r="I26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="7" t="s">
-        <v>220</v>
+      <c r="J26" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>32</v>
@@ -2275,8 +2272,8 @@
       <c r="I27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="7" t="s">
-        <v>220</v>
+      <c r="J27" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>32</v>
@@ -2310,8 +2307,8 @@
       <c r="I28" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="7" t="s">
-        <v>220</v>
+      <c r="J28" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>32</v>
@@ -2343,8 +2340,8 @@
       <c r="I29" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J29" s="7" t="s">
-        <v>220</v>
+      <c r="J29" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>32</v>
@@ -2374,8 +2371,8 @@
         <v>27</v>
       </c>
       <c r="I30" s="5"/>
-      <c r="J30" s="7" t="s">
-        <v>220</v>
+      <c r="J30" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>32</v>
@@ -2407,8 +2404,8 @@
       <c r="I31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J31" s="7" t="s">
-        <v>220</v>
+      <c r="J31" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>32</v>
@@ -2438,8 +2435,8 @@
         <v>147</v>
       </c>
       <c r="I32" s="5"/>
-      <c r="J32" s="7" t="s">
-        <v>220</v>
+      <c r="J32" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K32" s="5" t="s">
         <v>32</v>
@@ -2469,8 +2466,8 @@
         <v>35</v>
       </c>
       <c r="I33" s="5"/>
-      <c r="J33" s="7" t="s">
-        <v>220</v>
+      <c r="J33" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K33" s="5" t="s">
         <v>32</v>
@@ -2502,8 +2499,8 @@
       <c r="I34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J34" s="7" t="s">
-        <v>220</v>
+      <c r="J34" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K34" s="5" t="s">
         <v>32</v>
@@ -2535,8 +2532,8 @@
       <c r="I35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="7" t="s">
-        <v>220</v>
+      <c r="J35" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K35" s="5" t="s">
         <v>32</v>
@@ -2566,8 +2563,8 @@
         <v>148</v>
       </c>
       <c r="I36" s="5"/>
-      <c r="J36" s="7" t="s">
-        <v>220</v>
+      <c r="J36" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>32</v>
@@ -2597,8 +2594,8 @@
         <v>27</v>
       </c>
       <c r="I37" s="5"/>
-      <c r="J37" s="7" t="s">
-        <v>220</v>
+      <c r="J37" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>32</v>
@@ -2630,8 +2627,8 @@
       <c r="I38" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="J38" s="7" t="s">
-        <v>220</v>
+      <c r="J38" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>32</v>
@@ -2657,8 +2654,8 @@
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
-      <c r="J39" s="7" t="s">
-        <v>220</v>
+      <c r="J39" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>32</v>
@@ -2684,8 +2681,8 @@
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
-      <c r="J40" s="7" t="s">
-        <v>220</v>
+      <c r="J40" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>32</v>
@@ -2715,8 +2712,8 @@
         <v>147</v>
       </c>
       <c r="I41" s="5"/>
-      <c r="J41" s="7" t="s">
-        <v>220</v>
+      <c r="J41" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>32</v>
@@ -2748,8 +2745,8 @@
       <c r="I42" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="7" t="s">
-        <v>220</v>
+      <c r="J42" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>32</v>
@@ -2781,8 +2778,8 @@
       <c r="I43" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="J43" s="7" t="s">
-        <v>220</v>
+      <c r="J43" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>32</v>
@@ -2808,8 +2805,8 @@
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
-      <c r="J44" s="7" t="s">
-        <v>220</v>
+      <c r="J44" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>32</v>
@@ -2841,8 +2838,8 @@
       <c r="I45" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J45" s="7" t="s">
-        <v>220</v>
+      <c r="J45" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>32</v>
@@ -2870,8 +2867,8 @@
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
-      <c r="J46" s="7" t="s">
-        <v>220</v>
+      <c r="J46" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>32</v>
@@ -2901,8 +2898,8 @@
         <v>19</v>
       </c>
       <c r="I47" s="5"/>
-      <c r="J47" s="7" t="s">
-        <v>220</v>
+      <c r="J47" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K47" s="5" t="s">
         <v>32</v>
@@ -2932,8 +2929,8 @@
         <v>25</v>
       </c>
       <c r="I48" s="5"/>
-      <c r="J48" s="7" t="s">
-        <v>220</v>
+      <c r="J48" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K48" s="5" t="s">
         <v>32</v>
@@ -2965,15 +2962,15 @@
       <c r="I49" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="J49" s="7" t="s">
-        <v>220</v>
+      <c r="J49" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K49" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="8" t="s">
         <v>181</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -2998,8 +2995,8 @@
       <c r="I50" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J50" s="7" t="s">
-        <v>220</v>
+      <c r="J50" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K50" s="5" t="s">
         <v>32</v>
@@ -3031,8 +3028,8 @@
       <c r="I51" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J51" s="7" t="s">
-        <v>220</v>
+      <c r="J51" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K51" s="5" t="s">
         <v>32</v>
@@ -3064,8 +3061,8 @@
       <c r="I52" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J52" s="7" t="s">
-        <v>220</v>
+      <c r="J52" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K52" s="5" t="s">
         <v>32</v>
@@ -3097,8 +3094,8 @@
       <c r="I53" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J53" s="7" t="s">
-        <v>220</v>
+      <c r="J53" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K53" s="5" t="s">
         <v>32</v>
@@ -3130,8 +3127,8 @@
       <c r="I54" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J54" s="7" t="s">
-        <v>220</v>
+      <c r="J54" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K54" s="5" t="s">
         <v>32</v>
@@ -3161,8 +3158,8 @@
         <v>25</v>
       </c>
       <c r="I55" s="5"/>
-      <c r="J55" s="7" t="s">
-        <v>220</v>
+      <c r="J55" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K55" s="5" t="s">
         <v>32</v>
@@ -3194,8 +3191,8 @@
       <c r="I56" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J56" s="7" t="s">
-        <v>220</v>
+      <c r="J56" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K56" s="5" t="s">
         <v>32</v>
@@ -3229,8 +3226,8 @@
       <c r="I57" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J57" s="7" t="s">
-        <v>220</v>
+      <c r="J57" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K57" s="5" t="s">
         <v>32</v>
@@ -3262,8 +3259,8 @@
       <c r="I58" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="J58" s="7" t="s">
-        <v>220</v>
+      <c r="J58" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K58" s="5" t="s">
         <v>32</v>
@@ -3295,8 +3292,8 @@
       <c r="I59" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J59" s="7" t="s">
-        <v>220</v>
+      <c r="J59" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K59" s="5" t="s">
         <v>32</v>
@@ -3328,8 +3325,8 @@
       <c r="I60" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J60" s="7" t="s">
-        <v>220</v>
+      <c r="J60" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K60" s="5" t="s">
         <v>32</v>
@@ -3357,8 +3354,8 @@
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
-      <c r="J61" s="7" t="s">
-        <v>220</v>
+      <c r="J61" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K61" s="5" t="s">
         <v>32</v>
@@ -3390,8 +3387,8 @@
       <c r="I62" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="J62" s="7" t="s">
-        <v>220</v>
+      <c r="J62" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K62" s="5" t="s">
         <v>32</v>
@@ -3423,8 +3420,8 @@
         <v>138</v>
       </c>
       <c r="I63" s="5"/>
-      <c r="J63" s="7" t="s">
-        <v>220</v>
+      <c r="J63" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K63" s="5" t="s">
         <v>32</v>
@@ -3456,8 +3453,8 @@
       <c r="I64" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J64" s="7" t="s">
-        <v>220</v>
+      <c r="J64" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K64" s="5" t="s">
         <v>32</v>
@@ -3489,8 +3486,8 @@
       <c r="I65" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J65" s="7" t="s">
-        <v>220</v>
+      <c r="J65" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K65" s="5" t="s">
         <v>32</v>
@@ -3524,8 +3521,8 @@
       <c r="I66" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J66" s="7" t="s">
-        <v>220</v>
+      <c r="J66" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K66" s="5" t="s">
         <v>32</v>
@@ -3557,8 +3554,8 @@
       <c r="I67" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J67" s="7" t="s">
-        <v>220</v>
+      <c r="J67" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>32</v>
@@ -3590,8 +3587,8 @@
       <c r="I68" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J68" s="7" t="s">
-        <v>220</v>
+      <c r="J68" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K68" s="5" t="s">
         <v>32</v>
@@ -3623,8 +3620,8 @@
       <c r="I69" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J69" s="7" t="s">
-        <v>220</v>
+      <c r="J69" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K69" s="5" t="s">
         <v>32</v>
@@ -3656,8 +3653,8 @@
       <c r="I70" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J70" s="7" t="s">
-        <v>220</v>
+      <c r="J70" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K70" s="5" t="s">
         <v>32</v>
@@ -3689,8 +3686,8 @@
       <c r="I71" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="J71" s="7" t="s">
-        <v>220</v>
+      <c r="J71" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K71" s="5" t="s">
         <v>32</v>
@@ -3722,8 +3719,8 @@
       <c r="I72" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J72" s="7" t="s">
-        <v>220</v>
+      <c r="J72" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K72" s="5" t="s">
         <v>32</v>
@@ -3753,8 +3750,8 @@
         <v>166</v>
       </c>
       <c r="I73" s="5"/>
-      <c r="J73" s="7" t="s">
-        <v>220</v>
+      <c r="J73" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K73" s="5" t="s">
         <v>32</v>
@@ -3786,8 +3783,8 @@
       <c r="I74" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="J74" s="7" t="s">
-        <v>220</v>
+      <c r="J74" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K74" s="5" t="s">
         <v>32</v>
@@ -3819,8 +3816,8 @@
       <c r="I75" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J75" s="7" t="s">
-        <v>220</v>
+      <c r="J75" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K75" s="5" t="s">
         <v>32</v>
@@ -3852,8 +3849,8 @@
       <c r="I76" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J76" s="7" t="s">
-        <v>220</v>
+      <c r="J76" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>32</v>
@@ -3881,8 +3878,8 @@
       </c>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
-      <c r="J77" s="7" t="s">
-        <v>220</v>
+      <c r="J77" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K77" s="5" t="s">
         <v>32</v>
@@ -3912,8 +3909,8 @@
         <v>25</v>
       </c>
       <c r="I78" s="5"/>
-      <c r="J78" s="7" t="s">
-        <v>220</v>
+      <c r="J78" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K78" s="5" t="s">
         <v>32</v>
@@ -3945,8 +3942,8 @@
       <c r="I79" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="J79" s="7" t="s">
-        <v>220</v>
+      <c r="J79" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K79" s="5" t="s">
         <v>32</v>
@@ -3974,8 +3971,8 @@
       </c>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
-      <c r="J80" s="7" t="s">
-        <v>220</v>
+      <c r="J80" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K80" s="5" t="s">
         <v>32</v>
@@ -4007,8 +4004,8 @@
       <c r="I81" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J81" s="7" t="s">
-        <v>220</v>
+      <c r="J81" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K81" s="5" t="s">
         <v>32</v>
@@ -4036,8 +4033,8 @@
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
-      <c r="J82" s="7" t="s">
-        <v>220</v>
+      <c r="J82" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K82" s="5" t="s">
         <v>32</v>
@@ -4067,8 +4064,8 @@
         <v>146</v>
       </c>
       <c r="I83" s="5"/>
-      <c r="J83" s="7" t="s">
-        <v>220</v>
+      <c r="J83" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K83" s="5" t="s">
         <v>32</v>
@@ -4100,8 +4097,8 @@
       <c r="I84" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J84" s="7" t="s">
-        <v>220</v>
+      <c r="J84" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K84" s="5" t="s">
         <v>32</v>
@@ -4133,8 +4130,8 @@
       <c r="I85" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J85" s="7" t="s">
-        <v>220</v>
+      <c r="J85" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K85" s="5" t="s">
         <v>32</v>
@@ -4162,8 +4159,8 @@
       </c>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
-      <c r="J86" s="7" t="s">
-        <v>220</v>
+      <c r="J86" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K86" s="5" t="s">
         <v>32</v>
@@ -4193,8 +4190,8 @@
         <v>19</v>
       </c>
       <c r="I87" s="5"/>
-      <c r="J87" s="7" t="s">
-        <v>220</v>
+      <c r="J87" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K87" s="5" t="s">
         <v>32</v>
@@ -4226,8 +4223,8 @@
       <c r="I88" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J88" s="7" t="s">
-        <v>220</v>
+      <c r="J88" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K88" s="5" t="s">
         <v>32</v>
@@ -4259,8 +4256,8 @@
       <c r="I89" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="J89" s="7" t="s">
-        <v>220</v>
+      <c r="J89" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K89" s="5" t="s">
         <v>32</v>
@@ -4288,8 +4285,8 @@
       </c>
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
-      <c r="J90" s="7" t="s">
-        <v>220</v>
+      <c r="J90" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K90" s="5" t="s">
         <v>32</v>
@@ -4321,8 +4318,8 @@
       <c r="I91" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="J91" s="7" t="s">
-        <v>220</v>
+      <c r="J91" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K91" s="5" t="s">
         <v>32</v>
@@ -4352,8 +4349,8 @@
         <v>210</v>
       </c>
       <c r="I92" s="5"/>
-      <c r="J92" s="7" t="s">
-        <v>220</v>
+      <c r="J92" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K92" s="5" t="s">
         <v>32</v>
@@ -4385,8 +4382,8 @@
       <c r="I93" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="J93" s="7" t="s">
-        <v>220</v>
+      <c r="J93" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K93" s="5" t="s">
         <v>32</v>
@@ -4416,8 +4413,8 @@
         <v>147</v>
       </c>
       <c r="I94" s="5"/>
-      <c r="J94" s="7" t="s">
-        <v>220</v>
+      <c r="J94" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K94" s="5" t="s">
         <v>32</v>
@@ -4451,8 +4448,8 @@
       <c r="I95" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J95" s="7" t="s">
-        <v>220</v>
+      <c r="J95" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K95" s="5" t="s">
         <v>32</v>
@@ -4484,8 +4481,8 @@
       <c r="I96" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J96" s="7" t="s">
-        <v>220</v>
+      <c r="J96" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K96" s="5" t="s">
         <v>32</v>
@@ -4515,8 +4512,8 @@
         <v>196</v>
       </c>
       <c r="I97" s="5"/>
-      <c r="J97" s="7" t="s">
-        <v>220</v>
+      <c r="J97" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K97" s="5" t="s">
         <v>32</v>
@@ -4548,8 +4545,8 @@
       <c r="I98" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="J98" s="7" t="s">
-        <v>220</v>
+      <c r="J98" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K98" s="5" t="s">
         <v>32</v>
@@ -4581,8 +4578,8 @@
       <c r="I99" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J99" s="7" t="s">
-        <v>220</v>
+      <c r="J99" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K99" s="5" t="s">
         <v>32</v>
@@ -4612,8 +4609,8 @@
         <v>27</v>
       </c>
       <c r="I100" s="5"/>
-      <c r="J100" s="7" t="s">
-        <v>220</v>
+      <c r="J100" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K100" s="5" t="s">
         <v>32</v>
@@ -4645,8 +4642,8 @@
       <c r="I101" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="J101" s="7" t="s">
-        <v>220</v>
+      <c r="J101" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K101" s="5" t="s">
         <v>32</v>
@@ -4680,43 +4677,43 @@
       <c r="I102" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J102" s="7" t="s">
+      <c r="J102" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="K102" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E103" s="9">
+        <v>11</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H103" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="K102" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B103" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="D103" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E103" s="10">
-        <v>11</v>
-      </c>
-      <c r="F103" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="G103" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H103" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I103" s="10"/>
-      <c r="J103" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="K103" s="10" t="s">
+      <c r="K103" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4744,8 +4741,8 @@
         <v>198</v>
       </c>
       <c r="I104" s="5"/>
-      <c r="J104" s="7" t="s">
-        <v>220</v>
+      <c r="J104" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K104" s="5" t="s">
         <v>32</v>
@@ -4777,8 +4774,8 @@
       <c r="I105" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="J105" s="7" t="s">
-        <v>220</v>
+      <c r="J105" s="12" t="s">
+        <v>223</v>
       </c>
       <c r="K105" s="5" t="s">
         <v>32</v>
@@ -4789,7 +4786,7 @@
         <v>209</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>214</v>
@@ -4810,43 +4807,43 @@
       <c r="I106" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J106" s="5" t="s">
+      <c r="J106" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="K106" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B107" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="K106" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B107" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C107" s="10" t="s">
+      <c r="C107" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="D107" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E107" s="10">
+      <c r="D107" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E107" s="9">
         <v>45</v>
       </c>
-      <c r="F107" s="10"/>
-      <c r="G107" s="10" t="s">
+      <c r="F107" s="9"/>
+      <c r="G107" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H107" s="10" t="s">
+      <c r="H107" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I107" s="10" t="s">
+      <c r="I107" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J107" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="K107" s="10" t="s">
+      <c r="J107" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="K107" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4855,7 +4852,7 @@
         <v>172</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>30</v>
@@ -4874,17 +4871,19 @@
         <v>23</v>
       </c>
       <c r="I108" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="J108" s="5"/>
+        <v>226</v>
+      </c>
+      <c r="J108" s="12" t="s">
+        <v>223</v>
+      </c>
       <c r="K108" s="5"/>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B109" s="12" t="s">
-        <v>228</v>
+      <c r="B109" s="11" t="s">
+        <v>227</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>29</v>
@@ -4905,7 +4904,9 @@
       <c r="I109" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="J109" s="5"/>
+      <c r="J109" s="12" t="s">
+        <v>223</v>
+      </c>
       <c r="K109" s="5"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -5035,7 +5036,7 @@
       <formula>$K$62 ="YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:K108 C109:K109 B110:K113">
+  <conditionalFormatting sqref="B110:K113 B2:K108 C109:K109">
     <cfRule type="expression" dxfId="0" priority="3">
       <formula>$K$2="YES"</formula>
     </cfRule>

</xml_diff>